<commit_message>
ny db update eliteserine
</commit_message>
<xml_diff>
--- a/stored_data/eliteserien/R6-R20.xlsx
+++ b/stored_data/eliteserien/R6-R20.xlsx
@@ -240,18 +240,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -722,273 +715,273 @@
   </cellStyleXfs>
   <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1207,7 +1200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V982"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
@@ -1301,22 +1294,22 @@
       <c r="P2" s="12">
         <v>15</v>
       </c>
-      <c r="Q2" s="105">
+      <c r="Q2" s="104">
         <v>16</v>
       </c>
       <c r="R2" s="12">
         <v>17</v>
       </c>
-      <c r="S2" s="105">
+      <c r="S2" s="104">
         <v>18</v>
       </c>
-      <c r="T2" s="105">
+      <c r="T2" s="104">
         <v>19</v>
       </c>
-      <c r="U2" s="105">
+      <c r="U2" s="104">
         <v>20</v>
       </c>
-      <c r="V2" s="105">
+      <c r="V2" s="104">
         <v>21</v>
       </c>
     </row>
@@ -1364,23 +1357,23 @@
       <c r="O3" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="91"/>
-      <c r="Q3" s="102" t="s">
+      <c r="P3" s="107"/>
+      <c r="Q3" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="92" t="s">
+      <c r="R3" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="96" t="s">
+      <c r="S3" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="97" t="s">
+      <c r="T3" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="98" t="s">
+      <c r="U3" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="100" t="s">
+      <c r="V3" s="91" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1415,40 +1408,40 @@
       <c r="J4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="93" t="s">
+      <c r="K4" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="94" t="s">
+      <c r="L4" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="94" t="s">
+      <c r="M4" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="95" t="s">
+      <c r="N4" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="95" t="s">
+      <c r="O4" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="94" t="s">
+      <c r="P4" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="104" t="s">
+      <c r="Q4" s="94" t="s">
         <v>24</v>
       </c>
       <c r="R4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="96" t="s">
+      <c r="S4" s="97" t="s">
         <v>4</v>
       </c>
       <c r="T4" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="U4" s="94" t="s">
+      <c r="U4" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="V4" s="96" t="s">
+      <c r="V4" s="97" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1483,40 +1476,40 @@
       <c r="J5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="96" t="s">
+      <c r="K5" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="97" t="s">
+      <c r="L5" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="97" t="s">
+      <c r="M5" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="98" t="s">
+      <c r="N5" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="99" t="s">
+      <c r="O5" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="97" t="s">
+      <c r="P5" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="96" t="s">
+      <c r="Q5" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="97" t="s">
+      <c r="R5" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="S5" s="96" t="s">
+      <c r="S5" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="T5" s="99" t="s">
+      <c r="T5" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="U5" s="98" t="s">
+      <c r="U5" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="V5" s="100" t="s">
+      <c r="V5" s="96" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1551,38 +1544,38 @@
       <c r="J6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="100" t="s">
+      <c r="K6" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="97" t="s">
+      <c r="L6" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="98" t="s">
+      <c r="M6" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="98" t="s">
+      <c r="N6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="O6" s="99" t="s">
+      <c r="O6" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="97" t="s">
+      <c r="P6" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="Q6" s="107"/>
-      <c r="R6" s="95" t="s">
+      <c r="Q6" s="108"/>
+      <c r="R6" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="96" t="s">
+      <c r="S6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="T6" s="97" t="s">
+      <c r="T6" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="98" t="s">
+      <c r="U6" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="V6" s="96" t="s">
+      <c r="V6" s="97" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1617,40 +1610,40 @@
       <c r="J7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="102" t="s">
+      <c r="K7" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="97" t="s">
+      <c r="L7" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="103" t="s">
+      <c r="M7" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="N7" s="97" t="s">
+      <c r="N7" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="99" t="s">
+      <c r="O7" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="P7" s="103" t="s">
+      <c r="P7" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="Q7" s="108" t="s">
+      <c r="Q7" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="R7" s="99" t="s">
+      <c r="R7" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="S7" s="100" t="s">
+      <c r="S7" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="T7" s="97" t="s">
+      <c r="T7" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="U7" s="99" t="s">
+      <c r="U7" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="96" t="s">
+      <c r="V7" s="97" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1685,40 +1678,40 @@
       <c r="J8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="96" t="s">
+      <c r="K8" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="99" t="s">
+      <c r="L8" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="98" t="s">
+      <c r="M8" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="99" t="s">
+      <c r="N8" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="98" t="s">
+      <c r="O8" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="P8" s="99" t="s">
+      <c r="P8" s="101" t="s">
         <v>8</v>
       </c>
       <c r="Q8" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="R8" s="97" t="s">
+      <c r="R8" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="S8" s="100" t="s">
+      <c r="S8" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="T8" s="99" t="s">
+      <c r="T8" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="U8" s="99" t="s">
+      <c r="U8" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="V8" s="100" t="s">
+      <c r="V8" s="96" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1751,38 +1744,38 @@
         <v>21</v>
       </c>
       <c r="J9" s="20"/>
-      <c r="K9" s="104" t="s">
+      <c r="K9" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="98" t="s">
+      <c r="L9" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="M9" s="95" t="s">
+      <c r="M9" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="98" t="s">
+      <c r="N9" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="98" t="s">
+      <c r="O9" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="P9" s="101"/>
-      <c r="Q9" s="96" t="s">
+      <c r="P9" s="105"/>
+      <c r="Q9" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="R9" s="95" t="s">
+      <c r="R9" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="S9" s="104" t="s">
+      <c r="S9" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="94" t="s">
+      <c r="T9" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="U9" s="94" t="s">
+      <c r="U9" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="V9" s="96" t="s">
+      <c r="V9" s="97" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1817,38 +1810,38 @@
       <c r="J10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="104" t="s">
+      <c r="K10" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="94" t="s">
+      <c r="L10" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="M10" s="95" t="s">
+      <c r="M10" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="95" t="s">
+      <c r="N10" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="O10" s="94" t="s">
+      <c r="O10" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="P10" s="95" t="s">
+      <c r="P10" s="103" t="s">
         <v>10</v>
       </c>
       <c r="Q10" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="R10" s="95" t="s">
+      <c r="R10" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="S10" s="106"/>
-      <c r="T10" s="95" t="s">
+      <c r="S10" s="108"/>
+      <c r="T10" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="U10" s="95" t="s">
+      <c r="U10" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="V10" s="96" t="s">
+      <c r="V10" s="97" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1883,38 +1876,38 @@
       <c r="J11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="100" t="s">
+      <c r="K11" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="98" t="s">
+      <c r="L11" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="99" t="s">
+      <c r="M11" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="97" t="s">
+      <c r="N11" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="O11" s="98" t="s">
+      <c r="O11" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="P11" s="98" t="s">
+      <c r="P11" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="96" t="s">
+      <c r="Q11" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="R11" s="99" t="s">
+      <c r="R11" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="S11" s="106"/>
-      <c r="T11" s="98" t="s">
+      <c r="S11" s="108"/>
+      <c r="T11" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="U11" s="98" t="s">
+      <c r="U11" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="V11" s="104" t="s">
+      <c r="V11" s="94" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1949,40 +1942,40 @@
       <c r="J12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="100" t="s">
+      <c r="K12" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="L12" s="95" t="s">
+      <c r="L12" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="99" t="s">
+      <c r="M12" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="N12" s="94" t="s">
+      <c r="N12" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="O12" s="98" t="s">
+      <c r="O12" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="P12" s="98" t="s">
+      <c r="P12" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="Q12" s="96" t="s">
+      <c r="Q12" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="R12" s="95" t="s">
+      <c r="R12" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="S12" s="96" t="s">
+      <c r="S12" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="T12" s="95" t="s">
+      <c r="T12" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="U12" s="98" t="s">
+      <c r="U12" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="V12" s="96" t="s">
+      <c r="V12" s="97" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2017,40 +2010,40 @@
       <c r="J13" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="102" t="s">
+      <c r="K13" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="L13" s="98" t="s">
+      <c r="L13" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="M13" s="99" t="s">
+      <c r="M13" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="N13" s="98" t="s">
+      <c r="N13" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="98" t="s">
+      <c r="O13" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="103" t="s">
+      <c r="P13" s="106" t="s">
         <v>68</v>
       </c>
-      <c r="Q13" s="100" t="s">
+      <c r="Q13" s="96" t="s">
         <v>33</v>
       </c>
       <c r="R13" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="S13" s="100" t="s">
+      <c r="S13" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="T13" s="97" t="s">
+      <c r="T13" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="U13" s="98" t="s">
+      <c r="U13" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="V13" s="96" t="s">
+      <c r="V13" s="97" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2085,40 +2078,40 @@
       <c r="J14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="104" t="s">
+      <c r="K14" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="95" t="s">
+      <c r="L14" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="M14" s="94" t="s">
+      <c r="M14" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="97" t="s">
+      <c r="N14" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="O14" s="95" t="s">
+      <c r="O14" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="P14" s="98" t="s">
+      <c r="P14" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="Q14" s="96" t="s">
+      <c r="Q14" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="R14" s="98" t="s">
+      <c r="R14" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="S14" s="96" t="s">
+      <c r="S14" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="T14" s="98" t="s">
+      <c r="T14" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="U14" s="97" t="s">
+      <c r="U14" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="V14" s="104" t="s">
+      <c r="V14" s="94" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2153,38 +2146,38 @@
       <c r="J15" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="100" t="s">
+      <c r="K15" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="L15" s="98" t="s">
+      <c r="L15" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="M15" s="98" t="s">
+      <c r="M15" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="95" t="s">
+      <c r="N15" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="O15" s="97" t="s">
+      <c r="O15" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="P15" s="95" t="s">
+      <c r="P15" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="Q15" s="100" t="s">
+      <c r="Q15" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="R15" s="98" t="s">
+      <c r="R15" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="S15" s="106"/>
-      <c r="T15" s="94" t="s">
+      <c r="S15" s="108"/>
+      <c r="T15" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="U15" s="98" t="s">
+      <c r="U15" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="V15" s="104" t="s">
+      <c r="V15" s="94" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2217,40 +2210,40 @@
       <c r="J16" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="104" t="s">
+      <c r="K16" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="98" t="s">
+      <c r="L16" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="M16" s="95" t="s">
+      <c r="M16" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="N16" s="97" t="s">
+      <c r="N16" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="O16" s="95" t="s">
+      <c r="O16" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="P16" s="98" t="s">
+      <c r="P16" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="Q16" s="108" t="s">
+      <c r="Q16" s="102" t="s">
         <v>70</v>
       </c>
-      <c r="R16" s="97" t="s">
+      <c r="R16" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="S16" s="104" t="s">
+      <c r="S16" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="T16" s="98" t="s">
+      <c r="T16" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="U16" s="98" t="s">
+      <c r="U16" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="V16" s="96" t="s">
+      <c r="V16" s="97" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2285,36 +2278,36 @@
       <c r="J17" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="K17" s="93" t="s">
+      <c r="K17" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="L17" s="95" t="s">
+      <c r="L17" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="M17" s="95" t="s">
+      <c r="M17" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="N17" s="98" t="s">
+      <c r="N17" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="O17" s="94" t="s">
+      <c r="O17" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="P17" s="98" t="s">
+      <c r="P17" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="Q17" s="107"/>
-      <c r="R17" s="95" t="s">
+      <c r="Q17" s="108"/>
+      <c r="R17" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="S17" s="106"/>
-      <c r="T17" s="95" t="s">
+      <c r="S17" s="108"/>
+      <c r="T17" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="U17" s="95" t="s">
+      <c r="U17" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="V17" s="96" t="s">
+      <c r="V17" s="97" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2347,38 +2340,38 @@
       <c r="J18" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="K18" s="96" t="s">
+      <c r="K18" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="98" t="s">
+      <c r="L18" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="M18" s="101"/>
-      <c r="N18" s="95" t="s">
+      <c r="M18" s="100"/>
+      <c r="N18" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="O18" s="97" t="s">
+      <c r="O18" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="P18" s="97" t="s">
+      <c r="P18" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="Q18" s="104" t="s">
+      <c r="Q18" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="R18" s="95" t="s">
+      <c r="R18" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="S18" s="96" t="s">
+      <c r="S18" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="T18" s="98" t="s">
+      <c r="T18" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="U18" s="97" t="s">
+      <c r="U18" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="V18" s="96" t="s">
+      <c r="V18" s="97" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>